<commit_message>
update prestador hpd name v0.2.24
</commit_message>
<xml_diff>
--- a/fhir/ig/hpd/StructureDefinition-Mencion.xlsx
+++ b/fhir/ig/hpd/StructureDefinition-Mencion.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.2.2</t>
+    <t>0.2.4</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-11-10T09:26:13-03:00</t>
+    <t>2023-11-10T16:01:52-03:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>